<commit_message>
decoder sizing spreadsheet - dynamic blocking stages
</commit_message>
<xml_diff>
--- a/DecoderSizings.xlsx
+++ b/DecoderSizings.xlsx
@@ -225,7 +225,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="#,##0.###############"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -256,13 +256,6 @@
       <color rgb="FF000000"/>
       <name val="Times New Roman"/>
       <family val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="12">
@@ -328,7 +321,8 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -341,9 +335,8 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -369,10 +362,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" xfId="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Bad" xfId="1" builtinId="27"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -674,9 +666,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B5:B6"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.85546875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
@@ -930,7 +920,8 @@
         <v>1</v>
       </c>
       <c r="L9" s="19">
-        <v>1</v>
+        <f>B3</f>
+        <v>1.1000000000000001</v>
       </c>
       <c r="M9" s="6">
         <f>B4</f>
@@ -991,40 +982,42 @@
       </c>
       <c r="D11" s="8">
         <f>((E11*D9)*D10)/$C$21</f>
-        <v>36.34634039017498</v>
+        <v>28.055466474231068</v>
       </c>
       <c r="E11" s="8">
         <f>((F11*E9)*E10)/$C$21</f>
-        <v>33.026411493961611</v>
+        <v>19.677729977167573</v>
       </c>
       <c r="F11" s="8">
         <f>((G11*F9)*F10)/$C$21</f>
-        <v>109.12629036595595</v>
+        <v>50.187990333036012</v>
       </c>
       <c r="G11" s="8">
         <f>((H11*G9)*G10)/$C$21</f>
-        <v>396.63412951581057</v>
+        <v>140.8047480197524</v>
       </c>
       <c r="H11" s="8">
         <f>(((J11*H9)*H10)+I11)/$C$21</f>
-        <v>1441.6199081742393</v>
+        <v>395.03428874807139</v>
       </c>
       <c r="I11" s="7">
         <v>732</v>
       </c>
       <c r="J11" s="8">
         <f>((K11*J9)*J10)/$B$21</f>
-        <v>281.73504934846045</v>
+        <v>23.517945275895165</v>
       </c>
       <c r="K11" s="8">
-        <f>((N11*K9)*K10)/$B$21</f>
-        <v>907.85631061876427</v>
+        <f>((L11*K9)*K10)/$B$21</f>
+        <v>76.691935609531939</v>
       </c>
       <c r="L11" s="8">
-        <v>20</v>
+        <f>((M11*L9)*L10)/$B$21</f>
+        <v>275.10134114146126</v>
       </c>
       <c r="M11" s="8">
-        <v>32</v>
+        <f>((N11*M9)*M10)/$B$21</f>
+        <v>897.10449163011629</v>
       </c>
       <c r="N11" s="7">
         <v>3218</v>
@@ -1041,40 +1034,40 @@
       </c>
       <c r="D12" s="10">
         <f>FLOOR((D11*$E$4),1)</f>
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="E12" s="10">
         <f>FLOOR((E11*$E$3),1)</f>
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="F12" s="10">
         <f>FLOOR((F11*$E$4),1)</f>
-        <v>81</v>
+        <v>37</v>
       </c>
       <c r="G12" s="10">
         <f>FLOOR((G11*$E$4),1)</f>
-        <v>297</v>
+        <v>105</v>
       </c>
       <c r="H12" s="10">
         <f>FLOOR((H11*$E$4),1)</f>
-        <v>1081</v>
+        <v>296</v>
       </c>
       <c r="I12" s="10"/>
       <c r="J12" s="10">
         <f>FLOOR((J11*$E$3),1)</f>
-        <v>192</v>
+        <v>16</v>
       </c>
       <c r="K12" s="10">
         <f>FLOOR((K11*$E$4),1)</f>
-        <v>680</v>
+        <v>57</v>
       </c>
       <c r="L12" s="10">
         <f>FLOOR((L11*$E$3),1)</f>
-        <v>13</v>
+        <v>187</v>
       </c>
       <c r="M12" s="10">
         <f>FLOOR((M11*$E$4),1)</f>
-        <v>24</v>
+        <v>672</v>
       </c>
       <c r="N12" s="10"/>
     </row>
@@ -1089,40 +1082,40 @@
       </c>
       <c r="D13" s="10">
         <f t="shared" si="0"/>
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E13" s="10">
         <f t="shared" si="0"/>
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="F13" s="10">
         <f t="shared" si="0"/>
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="G13" s="10">
         <f t="shared" si="0"/>
-        <v>99</v>
+        <v>35</v>
       </c>
       <c r="H13" s="10">
         <f t="shared" si="0"/>
-        <v>360</v>
+        <v>99</v>
       </c>
       <c r="I13" s="10"/>
       <c r="J13" s="10">
         <f>FLOOR(J11,1)-J12</f>
-        <v>89</v>
+        <v>7</v>
       </c>
       <c r="K13" s="10">
         <f>FLOOR(K11,1)-K12</f>
-        <v>227</v>
+        <v>19</v>
       </c>
       <c r="L13" s="10">
         <f>FLOOR(L11,1)-L12</f>
-        <v>7</v>
+        <v>88</v>
       </c>
       <c r="M13" s="10">
         <f>FLOOR(M11,1)-M12</f>
-        <v>8</v>
+        <v>225</v>
       </c>
       <c r="N13" s="10"/>
     </row>
@@ -1160,7 +1153,7 @@
       </c>
       <c r="B17" s="13">
         <f>PRODUCT(C9:N9)</f>
-        <v>1.4520000000000002</v>
+        <v>1.5972000000000004</v>
       </c>
       <c r="C17" s="2">
         <f>PRODUCT(C9:H9)</f>
@@ -1171,7 +1164,7 @@
       </c>
       <c r="F17" s="2">
         <f>(2*$B$21+6*$C$21)*LN(2)</f>
-        <v>20.029896131616347</v>
+        <v>16.640711551889449</v>
       </c>
       <c r="H17" s="3" t="s">
         <v>32</v>
@@ -1216,14 +1209,14 @@
       </c>
       <c r="C19" s="2">
         <f>(($J$11*$H$10)+$I$11)/$B$11</f>
-        <v>218.32336623230697</v>
+        <v>46.178630183930103</v>
       </c>
       <c r="E19" s="3" t="s">
         <v>29</v>
       </c>
       <c r="F19" s="2">
         <f>SUM(F17:F18)</f>
-        <v>26.334069738809049</v>
+        <v>22.944885159082151</v>
       </c>
       <c r="H19" s="3" t="s">
         <v>34</v>
@@ -1239,18 +1232,18 @@
       </c>
       <c r="B20" s="2">
         <f>PRODUCT(B17:B19)</f>
-        <v>24920.192000000006</v>
+        <v>27412.211200000009</v>
       </c>
       <c r="C20" s="2">
         <f>PRODUCT(C17:C19)</f>
-        <v>2305.4947474131618</v>
+        <v>487.64633474230192</v>
       </c>
       <c r="E20" s="3" t="s">
         <v>35</v>
       </c>
       <c r="F20" s="2">
         <f>F19/(5*LN(2))</f>
-        <v>7.5984063637207866</v>
+        <v>6.6204944065549185</v>
       </c>
       <c r="H20" s="3" t="s">
         <v>36</v>
@@ -1266,11 +1259,11 @@
       </c>
       <c r="B21" s="2">
         <f>POWER(B20,(1/K7))</f>
-        <v>3.5446137922494803</v>
+        <v>3.587096074117984</v>
       </c>
       <c r="C21" s="2">
         <f>POWER(C20,(1/H7))</f>
-        <v>3.634634039017496</v>
+        <v>2.805546647423105</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
@@ -1322,22 +1315,22 @@
       </c>
       <c r="B25" s="2">
         <f>FLOOR(K11,1)</f>
-        <v>907</v>
+        <v>76</v>
       </c>
       <c r="C25" s="2">
         <f t="shared" ref="C25:D25" si="1">FLOOR(L11,1)</f>
-        <v>20</v>
+        <v>275</v>
       </c>
       <c r="D25" s="2">
         <f t="shared" si="1"/>
-        <v>32</v>
+        <v>897</v>
       </c>
       <c r="E25" s="2">
         <v>0</v>
       </c>
       <c r="F25" s="2">
         <f t="shared" ref="F25:F27" si="2">SUM(B25:E25)</f>
-        <v>959</v>
+        <v>1248</v>
       </c>
     </row>
     <row r="26" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1346,23 +1339,23 @@
       </c>
       <c r="B26" s="2">
         <f>FLOOR(J11,1)*$H$3</f>
-        <v>404.64</v>
+        <v>33.119999999999997</v>
       </c>
       <c r="C26" s="2">
         <f>FLOOR(K11,1)*$H$4</f>
-        <v>777.29899999999998</v>
+        <v>65.132000000000005</v>
       </c>
       <c r="D26" s="2">
         <f>FLOOR(L11,1)*$H$3</f>
-        <v>28.799999999999997</v>
+        <v>396</v>
       </c>
       <c r="E26" s="2">
         <f>FLOOR(M11,1)*$H$4</f>
-        <v>27.423999999999999</v>
+        <v>768.72900000000004</v>
       </c>
       <c r="F26" s="2">
         <f t="shared" si="2"/>
-        <v>1238.1629999999998</v>
+        <v>1262.981</v>
       </c>
     </row>
     <row r="27" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1371,23 +1364,23 @@
       </c>
       <c r="B27" s="2">
         <f>SUM(B24:B26)</f>
-        <v>1311.6399999999999</v>
+        <v>109.12</v>
       </c>
       <c r="C27" s="2">
         <f t="shared" ref="C27:E27" si="3">SUM(C24:C26)</f>
-        <v>797.29899999999998</v>
+        <v>340.13200000000001</v>
       </c>
       <c r="D27" s="2">
         <f t="shared" si="3"/>
-        <v>60.8</v>
+        <v>1293</v>
       </c>
       <c r="E27" s="2">
         <f t="shared" si="3"/>
-        <v>831.92399999999998</v>
+        <v>1573.229</v>
       </c>
       <c r="F27" s="16">
         <f t="shared" si="2"/>
-        <v>3001.663</v>
+        <v>3315.4809999999998</v>
       </c>
       <c r="G27" s="16" t="s">
         <v>41</v>
@@ -1397,7 +1390,7 @@
       <c r="A28" s="14"/>
       <c r="F28" s="16">
         <f>F27*$N$2*$N$3</f>
-        <v>92.451220399999997</v>
+        <v>102.11681479999999</v>
       </c>
       <c r="G28" s="16" t="s">
         <v>42</v>
@@ -1409,7 +1402,7 @@
       </c>
       <c r="B29" s="16">
         <f>F28*$N$5*($N$4^2)</f>
-        <v>92.451220399999997</v>
+        <v>102.11681479999999</v>
       </c>
       <c r="C29" s="16" t="s">
         <v>45</v>

</xml_diff>

<commit_message>
decoder sizing spreadsheet - fixed formulas
</commit_message>
<xml_diff>
--- a/DecoderSizings.xlsx
+++ b/DecoderSizings.xlsx
@@ -666,7 +666,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F22" sqref="F22"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.85546875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
@@ -978,46 +980,46 @@
       </c>
       <c r="C11" s="8">
         <f>((D11*C9)*C10)/$C$21</f>
-        <v>12.000000000000007</v>
+        <v>11.999999999999995</v>
       </c>
       <c r="D11" s="8">
         <f>((E11*D9)*D10)/$C$21</f>
-        <v>28.055466474231068</v>
+        <v>30.35354180178415</v>
       </c>
       <c r="E11" s="8">
         <f>((F11*E9)*E10)/$C$21</f>
-        <v>19.677729977167573</v>
+        <v>23.033437497816454</v>
       </c>
       <c r="F11" s="8">
         <f>((G11*F9)*F10)/$C$21</f>
-        <v>50.187990333036012</v>
+        <v>63.558764357159497</v>
       </c>
       <c r="G11" s="8">
         <f>((H11*G9)*G10)/$C$21</f>
-        <v>140.8047480197524</v>
+        <v>192.92336107847899</v>
       </c>
       <c r="H11" s="8">
         <f>(((J11*H9)*H10)+I11)/$C$21</f>
-        <v>395.03428874807139</v>
+        <v>585.59073050363111</v>
       </c>
       <c r="I11" s="7">
         <v>732</v>
       </c>
       <c r="J11" s="8">
         <f>((K11*J9)*J10)/$B$21</f>
-        <v>23.517945275895165</v>
+        <v>65.342204481745569</v>
       </c>
       <c r="K11" s="8">
         <f>((L11*K9)*K10)/$B$21</f>
-        <v>76.691935609531939</v>
+        <v>165.04239002663363</v>
       </c>
       <c r="L11" s="8">
         <f>((M11*L9)*L10)/$B$21</f>
-        <v>275.10134114146126</v>
+        <v>458.55339277150404</v>
       </c>
       <c r="M11" s="8">
         <f>((N11*M9)*M10)/$B$21</f>
-        <v>897.10449163011629</v>
+        <v>1158.2215276953714</v>
       </c>
       <c r="N11" s="7">
         <v>3218</v>
@@ -1034,40 +1036,40 @@
       </c>
       <c r="D12" s="10">
         <f>FLOOR((D11*$E$4),1)</f>
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E12" s="10">
         <f>FLOOR((E11*$E$3),1)</f>
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="F12" s="10">
         <f>FLOOR((F11*$E$4),1)</f>
-        <v>37</v>
+        <v>47</v>
       </c>
       <c r="G12" s="10">
         <f>FLOOR((G11*$E$4),1)</f>
-        <v>105</v>
+        <v>144</v>
       </c>
       <c r="H12" s="10">
         <f>FLOOR((H11*$E$4),1)</f>
-        <v>296</v>
+        <v>439</v>
       </c>
       <c r="I12" s="10"/>
       <c r="J12" s="10">
         <f>FLOOR((J11*$E$3),1)</f>
-        <v>16</v>
+        <v>44</v>
       </c>
       <c r="K12" s="10">
         <f>FLOOR((K11*$E$4),1)</f>
-        <v>57</v>
+        <v>123</v>
       </c>
       <c r="L12" s="10">
         <f>FLOOR((L11*$E$3),1)</f>
-        <v>187</v>
+        <v>313</v>
       </c>
       <c r="M12" s="10">
         <f>FLOOR((M11*$E$4),1)</f>
-        <v>672</v>
+        <v>868</v>
       </c>
       <c r="N12" s="10"/>
     </row>
@@ -1082,40 +1084,40 @@
       </c>
       <c r="D13" s="10">
         <f t="shared" si="0"/>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E13" s="10">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="F13" s="10">
         <f t="shared" si="0"/>
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="G13" s="10">
         <f t="shared" si="0"/>
-        <v>35</v>
+        <v>48</v>
       </c>
       <c r="H13" s="10">
         <f t="shared" si="0"/>
-        <v>99</v>
+        <v>146</v>
       </c>
       <c r="I13" s="10"/>
       <c r="J13" s="10">
         <f>FLOOR(J11,1)-J12</f>
-        <v>7</v>
+        <v>21</v>
       </c>
       <c r="K13" s="10">
         <f>FLOOR(K11,1)-K12</f>
-        <v>19</v>
+        <v>42</v>
       </c>
       <c r="L13" s="10">
         <f>FLOOR(L11,1)-L12</f>
-        <v>88</v>
+        <v>145</v>
       </c>
       <c r="M13" s="10">
         <f>FLOOR(M11,1)-M12</f>
-        <v>225</v>
+        <v>290</v>
       </c>
       <c r="N13" s="10"/>
     </row>
@@ -1163,8 +1165,8 @@
         <v>30</v>
       </c>
       <c r="F17" s="2">
-        <f>(2*$B$21+6*$C$21)*LN(2)</f>
-        <v>16.640711551889449</v>
+        <f>((M7-H7)*$B$21+H7*$C$21)*LN(2)</f>
+        <v>20.327037212308316</v>
       </c>
       <c r="H17" s="3" t="s">
         <v>32</v>
@@ -1189,8 +1191,8 @@
         <v>31</v>
       </c>
       <c r="F18" s="2">
-        <f>(1*$H$2+2*$H$3+5*$H$4)*LN(2)</f>
-        <v>6.3041736071927019</v>
+        <f>(COUNTIF(C8:M8,"Nand3")*$H$2+COUNTIF(C8:M8,"Nand2")*$H$3+COUNTIF(C8:M8,"Inv")*$H$4)*LN(2)</f>
+        <v>7.8963326809388965</v>
       </c>
       <c r="H18" s="3" t="s">
         <v>33</v>
@@ -1209,14 +1211,14 @@
       </c>
       <c r="C19" s="2">
         <f>(($J$11*$H$10)+$I$11)/$B$11</f>
-        <v>46.178630183930103</v>
+        <v>74.061469654497046</v>
       </c>
       <c r="E19" s="3" t="s">
         <v>29</v>
       </c>
       <c r="F19" s="2">
         <f>SUM(F17:F18)</f>
-        <v>22.944885159082151</v>
+        <v>28.223369893247213</v>
       </c>
       <c r="H19" s="3" t="s">
         <v>34</v>
@@ -1236,14 +1238,14 @@
       </c>
       <c r="C20" s="2">
         <f>PRODUCT(C17:C19)</f>
-        <v>487.64633474230192</v>
+        <v>782.08911955148881</v>
       </c>
       <c r="E20" s="3" t="s">
         <v>35</v>
       </c>
       <c r="F20" s="2">
         <f>F19/(5*LN(2))</f>
-        <v>6.6204944065549185</v>
+        <v>8.1435431564325249</v>
       </c>
       <c r="H20" s="3" t="s">
         <v>36</v>
@@ -1258,12 +1260,12 @@
         <v>27</v>
       </c>
       <c r="B21" s="2">
-        <f>POWER(B20,(1/K7))</f>
-        <v>3.587096074117984</v>
+        <f>POWER(B20,(1/M7))</f>
+        <v>2.7783976752730326</v>
       </c>
       <c r="C21" s="2">
         <f>POWER(C20,(1/H7))</f>
-        <v>2.805546647423105</v>
+        <v>3.0353541801784161</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
@@ -1315,22 +1317,22 @@
       </c>
       <c r="B25" s="2">
         <f>FLOOR(K11,1)</f>
-        <v>76</v>
+        <v>165</v>
       </c>
       <c r="C25" s="2">
         <f t="shared" ref="C25:D25" si="1">FLOOR(L11,1)</f>
-        <v>275</v>
+        <v>458</v>
       </c>
       <c r="D25" s="2">
         <f t="shared" si="1"/>
-        <v>897</v>
+        <v>1158</v>
       </c>
       <c r="E25" s="2">
         <v>0</v>
       </c>
       <c r="F25" s="2">
         <f t="shared" ref="F25:F27" si="2">SUM(B25:E25)</f>
-        <v>1248</v>
+        <v>1781</v>
       </c>
     </row>
     <row r="26" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1339,23 +1341,23 @@
       </c>
       <c r="B26" s="2">
         <f>FLOOR(J11,1)*$H$3</f>
-        <v>33.119999999999997</v>
+        <v>93.6</v>
       </c>
       <c r="C26" s="2">
         <f>FLOOR(K11,1)*$H$4</f>
-        <v>65.132000000000005</v>
+        <v>141.405</v>
       </c>
       <c r="D26" s="2">
         <f>FLOOR(L11,1)*$H$3</f>
-        <v>396</v>
+        <v>659.52</v>
       </c>
       <c r="E26" s="2">
         <f>FLOOR(M11,1)*$H$4</f>
-        <v>768.72900000000004</v>
+        <v>992.40599999999995</v>
       </c>
       <c r="F26" s="2">
         <f t="shared" si="2"/>
-        <v>1262.981</v>
+        <v>1886.931</v>
       </c>
     </row>
     <row r="27" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1364,23 +1366,23 @@
       </c>
       <c r="B27" s="2">
         <f>SUM(B24:B26)</f>
-        <v>109.12</v>
+        <v>258.60000000000002</v>
       </c>
       <c r="C27" s="2">
         <f t="shared" ref="C27:E27" si="3">SUM(C24:C26)</f>
-        <v>340.13200000000001</v>
+        <v>599.40499999999997</v>
       </c>
       <c r="D27" s="2">
         <f t="shared" si="3"/>
-        <v>1293</v>
+        <v>1817.52</v>
       </c>
       <c r="E27" s="2">
         <f t="shared" si="3"/>
-        <v>1573.229</v>
+        <v>1796.9059999999999</v>
       </c>
       <c r="F27" s="16">
         <f t="shared" si="2"/>
-        <v>3315.4809999999998</v>
+        <v>4472.4310000000005</v>
       </c>
       <c r="G27" s="16" t="s">
         <v>41</v>
@@ -1390,7 +1392,7 @@
       <c r="A28" s="14"/>
       <c r="F28" s="16">
         <f>F27*$N$2*$N$3</f>
-        <v>102.11681479999999</v>
+        <v>137.75087479999999</v>
       </c>
       <c r="G28" s="16" t="s">
         <v>42</v>
@@ -1402,7 +1404,7 @@
       </c>
       <c r="B29" s="16">
         <f>F28*$N$5*($N$4^2)</f>
-        <v>102.11681479999999</v>
+        <v>137.75087479999999</v>
       </c>
       <c r="C29" s="16" t="s">
         <v>45</v>

</xml_diff>

<commit_message>
added the dummy signals
</commit_message>
<xml_diff>
--- a/DecoderSizings.xlsx
+++ b/DecoderSizings.xlsx
@@ -1,26 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="13530" yWindow="-90" windowWidth="14805" windowHeight="13770" tabRatio="390" activeTab="2"/>
+    <workbookView xWindow="13530" yWindow="-90" windowWidth="14805" windowHeight="13770" tabRatio="390" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="block" sheetId="1" r:id="rId1"/>
     <sheet name="block+s8" sheetId="2" r:id="rId2"/>
     <sheet name="block+resize" sheetId="3" r:id="rId3"/>
+    <sheet name="dummy_sae_sizing" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="__shared_1_0_2">SUM(#REF!)</definedName>
     <definedName name="__shared_1_0_3">SUM(#REF!)</definedName>
   </definedNames>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="78">
   <si>
     <t>Constants:</t>
   </si>
@@ -412,11 +413,11 @@
     <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="2" fontId="1" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -949,23 +950,23 @@
     <row r="6" spans="1:19" customFormat="1" ht="15" customHeight="1">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
-      <c r="C6" s="19" t="s">
+      <c r="C6" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="D6" s="19"/>
-      <c r="E6" s="19"/>
-      <c r="F6" s="19"/>
-      <c r="G6" s="19"/>
-      <c r="H6" s="19"/>
+      <c r="D6" s="21"/>
+      <c r="E6" s="21"/>
+      <c r="F6" s="21"/>
+      <c r="G6" s="21"/>
+      <c r="H6" s="21"/>
       <c r="I6" s="1"/>
-      <c r="J6" s="19" t="s">
+      <c r="J6" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="K6" s="19"/>
-      <c r="L6" s="19" t="s">
+      <c r="K6" s="21"/>
+      <c r="L6" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="M6" s="19"/>
+      <c r="M6" s="21"/>
       <c r="N6" s="1"/>
       <c r="S6">
         <v>20.327000000000002</v>
@@ -2109,22 +2110,22 @@
       </c>
     </row>
     <row r="6" spans="1:14" ht="15" customHeight="1">
-      <c r="C6" s="19" t="s">
+      <c r="C6" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="D6" s="19"/>
-      <c r="E6" s="19"/>
-      <c r="F6" s="19"/>
-      <c r="G6" s="19"/>
-      <c r="H6" s="19"/>
-      <c r="J6" s="19" t="s">
+      <c r="D6" s="21"/>
+      <c r="E6" s="21"/>
+      <c r="F6" s="21"/>
+      <c r="G6" s="21"/>
+      <c r="H6" s="21"/>
+      <c r="J6" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="K6" s="19"/>
-      <c r="L6" s="19" t="s">
+      <c r="K6" s="21"/>
+      <c r="L6" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="M6" s="19"/>
+      <c r="M6" s="21"/>
     </row>
     <row r="7" spans="1:14" ht="15" customHeight="1">
       <c r="A7" s="4" t="s">
@@ -2816,8 +2817,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMM33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20:F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -7998,22 +7999,22 @@
       <c r="AMM5"/>
     </row>
     <row r="6" spans="1:1027" ht="15" customHeight="1">
-      <c r="C6" s="19" t="s">
+      <c r="C6" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="D6" s="19"/>
-      <c r="E6" s="19"/>
-      <c r="F6" s="19"/>
-      <c r="G6" s="19"/>
-      <c r="H6" s="19"/>
-      <c r="J6" s="19" t="s">
+      <c r="D6" s="21"/>
+      <c r="E6" s="21"/>
+      <c r="F6" s="21"/>
+      <c r="G6" s="21"/>
+      <c r="H6" s="21"/>
+      <c r="J6" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="K6" s="19"/>
-      <c r="L6" s="19" t="s">
+      <c r="K6" s="21"/>
+      <c r="L6" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="M6" s="19"/>
+      <c r="M6" s="21"/>
       <c r="Q6"/>
       <c r="R6"/>
       <c r="S6"/>
@@ -17556,7 +17557,7 @@
       <c r="R15" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="S15" s="21">
+      <c r="S15" s="20">
         <f>SUM(C18:M18)</f>
         <v>1663.9532044425962</v>
       </c>
@@ -19641,47 +19642,47 @@
         <v>69</v>
       </c>
       <c r="C17" s="1">
-        <f>C16*C9</f>
+        <f t="shared" ref="C17:M17" si="3">C16*C9</f>
         <v>2.1600000000000006</v>
       </c>
       <c r="D17" s="1">
-        <f>D16*D9</f>
+        <f t="shared" si="3"/>
         <v>3.1111111111111112</v>
       </c>
       <c r="E17" s="1">
-        <f>E16*E9</f>
+        <f t="shared" si="3"/>
         <v>1.4692857142857145</v>
       </c>
       <c r="F17" s="1">
-        <f>F16*F9</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="G17" s="1">
-        <f>G16*G9</f>
+        <f t="shared" si="3"/>
         <v>2.3529411764705883</v>
       </c>
       <c r="H17" s="1">
-        <f>H16*H9</f>
+        <f t="shared" si="3"/>
         <v>23.9</v>
       </c>
       <c r="I17" s="1">
-        <f>I16*I9</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="J17" s="1">
-        <f>J16*J9</f>
+        <f t="shared" si="3"/>
         <v>2.1607142857142865</v>
       </c>
       <c r="K17" s="1">
-        <f>K16*K9</f>
+        <f t="shared" si="3"/>
         <v>1.6</v>
       </c>
       <c r="L17" s="1">
-        <f>L16*L9</f>
+        <f t="shared" si="3"/>
         <v>3.0250000000000008</v>
       </c>
       <c r="M17" s="1">
-        <f>M16*M9</f>
+        <f t="shared" si="3"/>
         <v>32.18</v>
       </c>
       <c r="N17" s="2"/>
@@ -20701,48 +20702,48 @@
       <c r="A18" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="C18" s="20">
+      <c r="C18" s="19">
         <f>C12-C13</f>
         <v>0</v>
       </c>
-      <c r="D18" s="20">
-        <f t="shared" ref="D18:M18" si="3">D12-D13</f>
+      <c r="D18" s="19">
+        <f t="shared" ref="D18:M18" si="4">D12-D13</f>
         <v>12.35354180178415</v>
       </c>
-      <c r="E18" s="20">
-        <f t="shared" si="3"/>
+      <c r="E18" s="19">
+        <f t="shared" si="4"/>
         <v>9.033437497816454</v>
       </c>
-      <c r="F18" s="20">
-        <f t="shared" si="3"/>
+      <c r="F18" s="19">
+        <f t="shared" si="4"/>
         <v>46.558764357159497</v>
       </c>
-      <c r="G18" s="20">
-        <f t="shared" si="3"/>
+      <c r="G18" s="19">
+        <f t="shared" si="4"/>
         <v>175.92336107847899</v>
       </c>
-      <c r="H18" s="20">
-        <f t="shared" si="3"/>
+      <c r="H18" s="19">
+        <f t="shared" si="4"/>
         <v>545.59073050363111</v>
       </c>
-      <c r="I18" s="20">
-        <f t="shared" si="3"/>
+      <c r="I18" s="19">
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="J18" s="20">
-        <f t="shared" si="3"/>
+      <c r="J18" s="19">
+        <f t="shared" si="4"/>
         <v>51.342204481745569</v>
       </c>
-      <c r="K18" s="20">
-        <f t="shared" si="3"/>
+      <c r="K18" s="19">
+        <f t="shared" si="4"/>
         <v>140.04239002663363</v>
       </c>
-      <c r="L18" s="20">
-        <f t="shared" si="3"/>
+      <c r="L18" s="19">
+        <f t="shared" si="4"/>
         <v>418.55339277150404</v>
       </c>
-      <c r="M18" s="20">
-        <f t="shared" si="3"/>
+      <c r="M18" s="19">
+        <f t="shared" si="4"/>
         <v>264.55538192384284</v>
       </c>
       <c r="N18" s="2"/>
@@ -32048,7 +32049,7 @@
         <v>25</v>
       </c>
       <c r="C29" s="1">
-        <f t="shared" ref="C29:D29" si="4">L13</f>
+        <f t="shared" ref="C29" si="5">L13</f>
         <v>40</v>
       </c>
       <c r="D29" s="1">
@@ -37248,4 +37249,635 @@
     <oddFooter>&amp;CPage &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:N25"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetData>
+    <row r="1" spans="1:14" ht="15">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
+      <c r="M1" s="1"/>
+      <c r="N1" s="1"/>
+    </row>
+    <row r="2" spans="1:14" ht="15">
+      <c r="A2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1">
+        <v>1.2</v>
+      </c>
+      <c r="C2" s="1"/>
+      <c r="D2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="1">
+        <f>3/(3+1.78)</f>
+        <v>0.62761506276150625</v>
+      </c>
+      <c r="F2" s="1"/>
+      <c r="G2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="H2" s="1">
+        <v>1.93</v>
+      </c>
+      <c r="I2" s="1"/>
+      <c r="J2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="K2" s="3">
+        <v>6.0170000000000003</v>
+      </c>
+      <c r="L2" s="1"/>
+      <c r="M2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="N2" s="3">
+        <v>1.4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" ht="15">
+      <c r="A3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="1">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="C3" s="1"/>
+      <c r="D3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="1">
+        <f>3/(3+1.39)</f>
+        <v>0.68337129840546706</v>
+      </c>
+      <c r="F3" s="1"/>
+      <c r="G3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H3" s="1">
+        <v>1.44</v>
+      </c>
+      <c r="I3" s="1"/>
+      <c r="J3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="K3" s="1">
+        <v>19.7</v>
+      </c>
+      <c r="L3" s="1"/>
+      <c r="M3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="N3" s="1">
+        <v>2.1999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" ht="15">
+      <c r="A4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="1">
+        <v>1</v>
+      </c>
+      <c r="C4" s="1"/>
+      <c r="D4" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" s="1">
+        <v>0.75</v>
+      </c>
+      <c r="F4" s="1"/>
+      <c r="G4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H4" s="1">
+        <v>0.85699999999999998</v>
+      </c>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+      <c r="K4" s="1"/>
+      <c r="L4" s="3"/>
+      <c r="M4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="N4" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" ht="15">
+      <c r="A5" s="1"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
+      <c r="K5" s="1"/>
+      <c r="L5" s="3"/>
+      <c r="M5" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="N5" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" ht="15">
+      <c r="A6" s="1"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" s="21"/>
+      <c r="E6" s="21"/>
+      <c r="F6" s="21"/>
+      <c r="G6" s="21"/>
+      <c r="H6" s="21"/>
+    </row>
+    <row r="7" spans="1:14" ht="14.25">
+      <c r="A7" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" s="4">
+        <v>0</v>
+      </c>
+      <c r="C7" s="4">
+        <v>1</v>
+      </c>
+      <c r="D7" s="4">
+        <v>2</v>
+      </c>
+      <c r="E7" s="4">
+        <v>3</v>
+      </c>
+      <c r="F7" s="4">
+        <v>4</v>
+      </c>
+      <c r="G7" s="4">
+        <v>5</v>
+      </c>
+      <c r="H7" s="4">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" ht="15">
+      <c r="A8" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="F8" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="G8" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="H8" s="6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" ht="15">
+      <c r="A9" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B9" s="6"/>
+      <c r="C9" s="6">
+        <f>B2</f>
+        <v>1.2</v>
+      </c>
+      <c r="D9" s="6">
+        <f>B4</f>
+        <v>1</v>
+      </c>
+      <c r="E9" s="6">
+        <f>B3</f>
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="F9" s="6">
+        <f>B4</f>
+        <v>1</v>
+      </c>
+      <c r="G9" s="6">
+        <f>B4</f>
+        <v>1</v>
+      </c>
+      <c r="H9" s="6">
+        <f>B4</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" ht="15">
+      <c r="A10" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="B10" s="6"/>
+      <c r="C10" s="1">
+        <v>1.93</v>
+      </c>
+      <c r="D10" s="1">
+        <v>0.85699999999999998</v>
+      </c>
+      <c r="E10" s="1">
+        <v>1.44</v>
+      </c>
+      <c r="F10" s="1">
+        <v>0.85699999999999998</v>
+      </c>
+      <c r="G10" s="1">
+        <v>0.85699999999999998</v>
+      </c>
+      <c r="H10" s="1">
+        <v>0.85699999999999998</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" ht="15">
+      <c r="A11" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B11" s="7">
+        <v>2</v>
+      </c>
+      <c r="C11" s="7">
+        <v>1</v>
+      </c>
+      <c r="D11" s="7">
+        <v>4</v>
+      </c>
+      <c r="E11" s="7">
+        <v>1</v>
+      </c>
+      <c r="F11" s="7">
+        <v>1</v>
+      </c>
+      <c r="G11" s="7">
+        <v>1</v>
+      </c>
+      <c r="H11" s="7">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" ht="15">
+      <c r="A12" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="B12" s="7">
+        <v>24</v>
+      </c>
+      <c r="C12" s="8">
+        <v>11.999999999999995</v>
+      </c>
+      <c r="D12" s="8">
+        <v>30.35354180178415</v>
+      </c>
+      <c r="E12" s="8">
+        <v>23.033437497816454</v>
+      </c>
+      <c r="F12" s="8">
+        <v>63.558764357159497</v>
+      </c>
+      <c r="G12" s="8">
+        <v>192.92336107847899</v>
+      </c>
+      <c r="H12" s="8">
+        <v>585.59073050363111</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" ht="15">
+      <c r="A13" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="B13" s="7">
+        <v>24</v>
+      </c>
+      <c r="C13" s="8">
+        <v>11.999999999999995</v>
+      </c>
+      <c r="D13" s="8">
+        <v>18</v>
+      </c>
+      <c r="E13" s="8">
+        <v>14</v>
+      </c>
+      <c r="F13" s="8">
+        <v>17</v>
+      </c>
+      <c r="G13" s="8">
+        <v>17</v>
+      </c>
+      <c r="H13" s="8">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" ht="15">
+      <c r="A14" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="B14" s="10"/>
+      <c r="C14" s="16">
+        <v>7</v>
+      </c>
+      <c r="D14" s="16">
+        <f>FLOOR((D13*$E$4),1)</f>
+        <v>13</v>
+      </c>
+      <c r="E14" s="16">
+        <f>FLOOR((E13*$E$3),1)</f>
+        <v>9</v>
+      </c>
+      <c r="F14" s="16">
+        <f>FLOOR((F13*$E$4),1)</f>
+        <v>12</v>
+      </c>
+      <c r="G14" s="16">
+        <f>FLOOR((G13*$E$4),1)</f>
+        <v>12</v>
+      </c>
+      <c r="H14" s="16">
+        <f>FLOOR((H13*$E$4),1)</f>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" ht="15">
+      <c r="A15" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="B15" s="10"/>
+      <c r="C15" s="16">
+        <v>5</v>
+      </c>
+      <c r="D15" s="16">
+        <f t="shared" ref="D15:H15" si="0">FLOOR(D13,1)-D14</f>
+        <v>5</v>
+      </c>
+      <c r="E15" s="16">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="F15" s="16">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="G15" s="16">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="H15" s="16">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" ht="15">
+      <c r="A16" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="B16" s="1"/>
+      <c r="C16" s="1">
+        <f>D13*C9*C11/C13</f>
+        <v>1.8000000000000007</v>
+      </c>
+      <c r="D16" s="1">
+        <f>E13*D9*D11/D13</f>
+        <v>3.1111111111111112</v>
+      </c>
+      <c r="E16" s="1">
+        <f>F13*E9*E11/E13</f>
+        <v>1.3357142857142859</v>
+      </c>
+      <c r="F16" s="1">
+        <f>G13*F9*F11/F13</f>
+        <v>1</v>
+      </c>
+      <c r="G16" s="1">
+        <f>H13*G9*G11/G13</f>
+        <v>2.3529411764705883</v>
+      </c>
+      <c r="H16" s="1">
+        <f>(I13+(J13*H11))*H9/H13</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="15">
+      <c r="A17" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="B17" s="1"/>
+      <c r="C17" s="1">
+        <f t="shared" ref="C17:H17" si="1">C16*C9</f>
+        <v>2.1600000000000006</v>
+      </c>
+      <c r="D17" s="1">
+        <f t="shared" si="1"/>
+        <v>3.1111111111111112</v>
+      </c>
+      <c r="E17" s="1">
+        <f t="shared" si="1"/>
+        <v>1.4692857142857145</v>
+      </c>
+      <c r="F17" s="1">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="G17" s="1">
+        <f t="shared" si="1"/>
+        <v>2.3529411764705883</v>
+      </c>
+      <c r="H17" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="15">
+      <c r="A18" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B18" s="1"/>
+      <c r="C18" s="19">
+        <f>C12-C13</f>
+        <v>0</v>
+      </c>
+      <c r="D18" s="19">
+        <f t="shared" ref="D18:H18" si="2">D12-D13</f>
+        <v>12.35354180178415</v>
+      </c>
+      <c r="E18" s="19">
+        <f t="shared" si="2"/>
+        <v>9.033437497816454</v>
+      </c>
+      <c r="F18" s="19">
+        <f t="shared" si="2"/>
+        <v>46.558764357159497</v>
+      </c>
+      <c r="G18" s="19">
+        <f t="shared" si="2"/>
+        <v>175.92336107847899</v>
+      </c>
+      <c r="H18" s="19">
+        <f t="shared" si="2"/>
+        <v>545.59073050363111</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="15">
+      <c r="A19" s="11"/>
+      <c r="B19" s="12"/>
+      <c r="C19" s="13"/>
+      <c r="D19" s="13"/>
+      <c r="E19" s="13"/>
+      <c r="F19" s="13"/>
+      <c r="G19" s="13"/>
+      <c r="H19" s="13"/>
+    </row>
+    <row r="20" spans="1:8" ht="15">
+      <c r="A20" s="2"/>
+      <c r="B20" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
+      <c r="F20" s="1"/>
+    </row>
+    <row r="21" spans="1:8" ht="15">
+      <c r="A21" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B21" s="14">
+        <f>PRODUCT(C9:N9)</f>
+        <v>1.32</v>
+      </c>
+      <c r="C21" s="1">
+        <f>PRODUCT(C9:H9)</f>
+        <v>1.32</v>
+      </c>
+      <c r="D21" s="1"/>
+      <c r="E21" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="F21" s="1" t="e">
+        <f>(1*C25*B2+4*C25*B4+1*C25*B3+2*B25*B3+2*B25*B4)*LN(2)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="15">
+      <c r="A22" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B22" s="1">
+        <f>PRODUCT(B11:N11)</f>
+        <v>128</v>
+      </c>
+      <c r="C22" s="1">
+        <f>PRODUCT(B11:G11)</f>
+        <v>8</v>
+      </c>
+      <c r="D22" s="1"/>
+      <c r="E22" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="F22" s="1">
+        <f>(COUNTIF(C8:M8,"Nand3")*$H$2*C9+COUNTIF(C8:M8,"Nand2")*$H$3*B3+COUNTIF(C8:M8,"Inv")*$H$4*B4)*LN(2)</f>
+        <v>5.0793825391432783</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="15">
+      <c r="A23" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B23" s="1">
+        <f>$N$13/$B$13</f>
+        <v>0</v>
+      </c>
+      <c r="C23" s="1">
+        <f>(($J$13*$H$11)+$I$13)/$B$13</f>
+        <v>0</v>
+      </c>
+      <c r="D23" s="1"/>
+      <c r="E23" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="F23" s="1" t="e">
+        <f>SUM(F21:F22)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="15">
+      <c r="A24" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B24" s="1">
+        <f>PRODUCT(B21:B23)</f>
+        <v>0</v>
+      </c>
+      <c r="C24" s="1">
+        <f>PRODUCT(C21:C23)</f>
+        <v>0</v>
+      </c>
+      <c r="D24" s="1"/>
+      <c r="E24" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="F24" s="1" t="e">
+        <f>F23/(5*LN(2))</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" ht="15">
+      <c r="A25" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B25" s="1" t="e">
+        <f>POWER(B24,(1/M7))</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C25" s="1">
+        <f>POWER(C24,(1/H7))</f>
+        <v>0</v>
+      </c>
+      <c r="D25" s="1"/>
+      <c r="E25" s="1"/>
+      <c r="F25" s="1" t="e">
+        <f>F24*21.2</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="C6:H6"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>